<commit_message>
Added Update and Delete in Food Items
</commit_message>
<xml_diff>
--- a/Final Outputs/Schema and Workflow/ITECC05 SCHEMA.xlsx
+++ b/Final Outputs/Schema and Workflow/ITECC05 SCHEMA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamp\Desktop\ITECC05\Final Output (ITECC05)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamp\Desktop\ITECC05\itek05_collab\Final Outputs\Schema and Workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D10530-F872-4696-8928-170EDF5F0F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593E4D5E-A084-4B6B-A21B-F5990C7B3799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="159">
   <si>
     <t>db_food_kiosk</t>
   </si>
@@ -34,36 +34,12 @@
     <t>GET</t>
   </si>
   <si>
-    <t>insertFood</t>
-  </si>
-  <si>
-    <t>addFood</t>
-  </si>
-  <si>
-    <t>modifyFood</t>
-  </si>
-  <si>
     <t>updateFood</t>
   </si>
   <si>
-    <t>fetchAllFood</t>
-  </si>
-  <si>
-    <t>getAllFood</t>
-  </si>
-  <si>
-    <t>fetchFoodById</t>
-  </si>
-  <si>
-    <t>getAllFoodById</t>
-  </si>
-  <si>
     <t>deleteFood</t>
   </si>
   <si>
-    <t>removeFood</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -244,33 +220,15 @@
     <t>updateStock</t>
   </si>
   <si>
-    <t>adjustStock</t>
-  </si>
-  <si>
     <t>/api/foods/stock/:id</t>
   </si>
   <si>
-    <t>toggleAvailability</t>
-  </si>
-  <si>
-    <t>setAvailability</t>
-  </si>
-  <si>
     <t>/api/foods/available/:id</t>
   </si>
   <si>
-    <t>fetchAllAvailableFood</t>
-  </si>
-  <si>
-    <t>fetchFoodByCategoryId</t>
-  </si>
-  <si>
     <t>getAvailableFood</t>
   </si>
   <si>
-    <t>getFoodByCategory</t>
-  </si>
-  <si>
     <t>/api/foods/available</t>
   </si>
   <si>
@@ -292,36 +250,15 @@
     <t>Categories</t>
   </si>
   <si>
-    <t>insertCategory</t>
-  </si>
-  <si>
-    <t>addCategory</t>
-  </si>
-  <si>
-    <t>fetchAllCategories</t>
-  </si>
-  <si>
-    <t>getAllCategories</t>
-  </si>
-  <si>
-    <t>fetchCategoryById</t>
-  </si>
-  <si>
     <t>getCategoryById</t>
   </si>
   <si>
-    <t>modifyCategory</t>
-  </si>
-  <si>
     <t>updateCategory</t>
   </si>
   <si>
     <t>deleteCategory</t>
   </si>
   <si>
-    <t>removeCategory</t>
-  </si>
-  <si>
     <t>/api/categories/</t>
   </si>
   <si>
@@ -334,12 +271,6 @@
     <t xml:space="preserve">PUT </t>
   </si>
   <si>
-    <t>fetchAllActiveCategories</t>
-  </si>
-  <si>
-    <t>getAllActiveCategories</t>
-  </si>
-  <si>
     <t>/api/categories/active</t>
   </si>
   <si>
@@ -518,6 +449,54 @@
   </si>
   <si>
     <t>orderDetailRoutes</t>
+  </si>
+  <si>
+    <t>getFoodById</t>
+  </si>
+  <si>
+    <t>getFoodByCategoryId</t>
+  </si>
+  <si>
+    <t>createFood</t>
+  </si>
+  <si>
+    <t>updateAvailability</t>
+  </si>
+  <si>
+    <t>getFood</t>
+  </si>
+  <si>
+    <t>store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update </t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>indexAvailable</t>
+  </si>
+  <si>
+    <t>indexByCategory</t>
+  </si>
+  <si>
+    <t>destroy</t>
+  </si>
+  <si>
+    <t>createCategory</t>
+  </si>
+  <si>
+    <t>getCategories</t>
+  </si>
+  <si>
+    <t>getActiveCategories</t>
+  </si>
+  <si>
+    <t>indexActive</t>
   </si>
 </sst>
 </file>
@@ -843,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +831,7 @@
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
     <col min="6" max="6" width="29.5703125" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" customWidth="1"/>
@@ -861,6 +840,9 @@
     <col min="10" max="10" width="25.85546875" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -870,110 +852,110 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" t="s">
+        <v>146</v>
+      </c>
+      <c r="K3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -981,19 +963,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="H6" t="s">
         <v>2</v>
@@ -1007,38 +989,38 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
       </c>
       <c r="D10">
         <v>100</v>
@@ -1047,22 +1029,22 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1">
         <v>10</v>
@@ -1071,30 +1053,30 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -1104,83 +1086,83 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="G17" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I17" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>91</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="F18" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="G18" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="I18" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I19" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1188,16 +1170,16 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
         <v>2</v>
@@ -1205,24 +1187,24 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D22">
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -1230,10 +1212,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1241,90 +1223,90 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F28" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H28" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" t="s">
         <v>48</v>
-      </c>
-      <c r="E29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F30" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G30" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1335,10 +1317,10 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F31" t="s">
         <v>2</v>
@@ -1346,24 +1328,24 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D33">
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D34">
         <v>100</v>
@@ -1371,10 +1353,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D35">
         <v>15</v>
@@ -1382,10 +1364,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
@@ -1393,81 +1375,81 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="D41" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="E41" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G41" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="D42" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="F42" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="D43" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="F43" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1478,18 +1460,18 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D46" s="1">
         <v>10</v>
@@ -1497,10 +1479,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D47" s="1">
         <v>20</v>
@@ -1508,32 +1490,32 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D50" s="1">
         <v>10</v>
@@ -1541,19 +1523,19 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
@@ -1561,74 +1543,74 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="C54" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D54" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F54" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="G54" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H54" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="C55" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="D55" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="E55" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="F55" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="G55" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H55" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="C56" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="D56" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="E56" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="F56" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="G56" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="H56" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -1636,35 +1618,35 @@
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F57" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D59" s="1">
         <v>10</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D60" s="1">
         <v>50</v>
@@ -1672,20 +1654,20 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="C61" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C62" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D62" s="1">
         <v>10</v>
@@ -1694,95 +1676,95 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C63" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B71" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="C71" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="D71" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="E71" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="F71" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G71" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="E72" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="F72" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G72" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="C73" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="D73" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="E73" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="F73" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G73" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -1801,52 +1783,52 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="C76" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D76" s="1">
         <v>10</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C77" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D77" s="1">
         <v>10</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C78" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D78" s="1">
         <v>10</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C79" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D79" s="1">
         <v>5</v>
@@ -1855,25 +1837,25 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="C80" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="C81" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added specialized methods for Food Items. Updated schema
</commit_message>
<xml_diff>
--- a/Final Outputs/Schema and Workflow/ITECC05 SCHEMA.xlsx
+++ b/Final Outputs/Schema and Workflow/ITECC05 SCHEMA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamp\Desktop\ITECC05\itek05_collab\Final Outputs\Schema and Workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593E4D5E-A084-4B6B-A21B-F5990C7B3799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4482FF00-4CF0-4F66-AB41-6DD52FCF6F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14955" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="151">
   <si>
     <t>db_food_kiosk</t>
   </si>
@@ -109,9 +109,6 @@
     <t xml:space="preserve">int </t>
   </si>
   <si>
-    <t>datetime</t>
-  </si>
-  <si>
     <t>total_amount</t>
   </si>
   <si>
@@ -121,36 +118,12 @@
     <t>10,2</t>
   </si>
   <si>
-    <t>insertCustomer</t>
-  </si>
-  <si>
-    <t>fetchAllCustomers</t>
-  </si>
-  <si>
-    <t>modifyCustomer</t>
-  </si>
-  <si>
-    <t>fetchAllCustomersById</t>
-  </si>
-  <si>
     <t>deleteCustomer</t>
   </si>
   <si>
-    <t>addCustomer</t>
-  </si>
-  <si>
     <t>updateCustomer</t>
   </si>
   <si>
-    <t>getAllCustomers</t>
-  </si>
-  <si>
-    <t>getAllCustomersById</t>
-  </si>
-  <si>
-    <t>removeCustomer</t>
-  </si>
-  <si>
     <t>foodRoute</t>
   </si>
   <si>
@@ -172,12 +145,6 @@
     <t>customersRoute</t>
   </si>
   <si>
-    <t>fetchAllOrder</t>
-  </si>
-  <si>
-    <t>fetchAllOrderById</t>
-  </si>
-  <si>
     <t>orderController</t>
   </si>
   <si>
@@ -196,9 +163,6 @@
     <t>Order Details</t>
   </si>
   <si>
-    <t>bool</t>
-  </si>
-  <si>
     <t>is_available</t>
   </si>
   <si>
@@ -307,51 +271,24 @@
     <t>expiry_date</t>
   </si>
   <si>
-    <t>percentage, fixes</t>
-  </si>
-  <si>
-    <t>5, 2</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
-    <t>insertDiscount</t>
-  </si>
-  <si>
-    <t>addDiscount</t>
-  </si>
-  <si>
     <t>/api/discounts/</t>
   </si>
   <si>
-    <t>fetchAllDiscounts</t>
-  </si>
-  <si>
-    <t>getAllDiscounts</t>
-  </si>
-  <si>
     <t>/api/discounts</t>
   </si>
   <si>
-    <t>fetchDiscountByCode</t>
-  </si>
-  <si>
     <t>/api/discounts/apply</t>
   </si>
   <si>
-    <t>fetchDiscountUsage</t>
-  </si>
-  <si>
     <t>getDiscountUsage</t>
   </si>
   <si>
     <t>/api/discounts/usage/:id</t>
   </si>
   <si>
-    <t>applyDiscounts</t>
-  </si>
-  <si>
     <t>discountModel</t>
   </si>
   <si>
@@ -361,9 +298,6 @@
     <t>discountRoutes</t>
   </si>
   <si>
-    <t>order_date_time</t>
-  </si>
-  <si>
     <t>discount_amount</t>
   </si>
   <si>
@@ -382,75 +316,15 @@
     <t>line_total</t>
   </si>
   <si>
-    <t>createNewOrder</t>
-  </si>
-  <si>
-    <t>submitOrder</t>
-  </si>
-  <si>
     <t>/api/orders</t>
   </si>
   <si>
-    <t>getDailyOrders</t>
-  </si>
-  <si>
-    <t>getAllOrderDetails</t>
-  </si>
-  <si>
-    <t>updateOrderStatus</t>
-  </si>
-  <si>
-    <t>changeOrderStatus</t>
-  </si>
-  <si>
-    <t>/api/orders/status/:id</t>
-  </si>
-  <si>
     <t>/api/orders/:id</t>
   </si>
   <si>
-    <t>fetchSalesByDate</t>
-  </si>
-  <si>
-    <t>getSales</t>
-  </si>
-  <si>
-    <t>/api/reports/sales</t>
-  </si>
-  <si>
     <t>orderRoute</t>
   </si>
   <si>
-    <t>insertOrderDetail</t>
-  </si>
-  <si>
-    <t>fetchDetailsByOrderId</t>
-  </si>
-  <si>
-    <t>modifyOrderDetail</t>
-  </si>
-  <si>
-    <t>deleteOrderDetail</t>
-  </si>
-  <si>
-    <t>updateOrderItem</t>
-  </si>
-  <si>
-    <t>removeOrderItem</t>
-  </si>
-  <si>
-    <t>/api/order-details/:detailId</t>
-  </si>
-  <si>
-    <t>orderDetailModel</t>
-  </si>
-  <si>
-    <t>orderDetailController</t>
-  </si>
-  <si>
-    <t>orderDetailRoutes</t>
-  </si>
-  <si>
     <t>getFoodById</t>
   </si>
   <si>
@@ -497,6 +371,108 @@
   </si>
   <si>
     <t>indexActive</t>
+  </si>
+  <si>
+    <t>createCustomer</t>
+  </si>
+  <si>
+    <t>getCustomers</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>getCustomersById</t>
+  </si>
+  <si>
+    <t>createDiscount</t>
+  </si>
+  <si>
+    <t>getDiscountByCode</t>
+  </si>
+  <si>
+    <t>getDiscounts</t>
+  </si>
+  <si>
+    <t>indexByCode</t>
+  </si>
+  <si>
+    <t>indexDiscountUsage</t>
+  </si>
+  <si>
+    <t>updateDiscount</t>
+  </si>
+  <si>
+    <t>deleteDiscount</t>
+  </si>
+  <si>
+    <t>createOrder</t>
+  </si>
+  <si>
+    <t>getOrder</t>
+  </si>
+  <si>
+    <t>getOrderById</t>
+  </si>
+  <si>
+    <t>deleteOrderStatus</t>
+  </si>
+  <si>
+    <t>indexById</t>
+  </si>
+  <si>
+    <t>updateOrder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELETE </t>
+  </si>
+  <si>
+    <t>createOrderDetail</t>
+  </si>
+  <si>
+    <t>getDetailByOrderId</t>
+  </si>
+  <si>
+    <t>indexByOrder</t>
+  </si>
+  <si>
+    <t>getDetailById</t>
+  </si>
+  <si>
+    <t>/api/orders/:order_id/details</t>
+  </si>
+  <si>
+    <t>/api/orders/orders_id/details</t>
+  </si>
+  <si>
+    <t>/api/orders/details/:id</t>
+  </si>
+  <si>
+    <t>updateDetail</t>
+  </si>
+  <si>
+    <t>/api/order/details/:id</t>
+  </si>
+  <si>
+    <t>deleteDetail</t>
+  </si>
+  <si>
+    <t>percentage, fixed</t>
+  </si>
+  <si>
+    <t>order_date</t>
+  </si>
+  <si>
+    <t>order_time</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT </t>
+  </si>
+  <si>
+    <t>NOT DONE</t>
   </si>
 </sst>
 </file>
@@ -820,18 +796,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
     <col min="6" max="6" width="29.5703125" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" customWidth="1"/>
@@ -852,22 +828,22 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -876,10 +852,10 @@
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="K3" t="s">
         <v>6</v>
@@ -890,31 +866,31 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="G4" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="J4" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="K4" t="s">
         <v>7</v>
@@ -931,31 +907,31 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="K5" t="s">
         <v>8</v>
       </c>
       <c r="L5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -969,10 +945,10 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G6" t="s">
         <v>2</v>
@@ -995,7 +971,7 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
@@ -1009,7 +985,7 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>19</v>
@@ -1047,36 +1023,38 @@
         <v>17</v>
       </c>
       <c r="D12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -1086,83 +1064,83 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>113</v>
       </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="F17" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="H17" t="s">
         <v>6</v>
       </c>
       <c r="I17" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="F18" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="G18" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
       <c r="H18" t="s">
         <v>7</v>
       </c>
       <c r="I18" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="H19" t="s">
         <v>8</v>
       </c>
       <c r="I19" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1170,16 +1148,16 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="G20" t="s">
         <v>2</v>
@@ -1212,101 +1190,96 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="E25" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" t="s">
         <v>33</v>
       </c>
-      <c r="C28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="F28" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G28" t="s">
         <v>6</v>
       </c>
       <c r="H28" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="F29" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="G29" t="s">
         <v>7</v>
       </c>
       <c r="H29" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G30" t="s">
         <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1314,19 +1287,19 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" t="s">
         <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" t="s">
-        <v>71</v>
       </c>
       <c r="F31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>25</v>
       </c>
@@ -1334,15 +1307,15 @@
         <v>17</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
         <v>20</v>
@@ -1351,7 +1324,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>26</v>
       </c>
@@ -1362,124 +1335,148 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" t="s">
+        <v>127</v>
+      </c>
+      <c r="H41" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" t="s">
+        <v>112</v>
+      </c>
+      <c r="H42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" t="s">
         <v>88</v>
       </c>
-      <c r="B41" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" t="s">
-        <v>104</v>
-      </c>
-      <c r="D41" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" t="s">
-        <v>106</v>
-      </c>
-      <c r="F41" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" t="s">
-        <v>102</v>
-      </c>
-      <c r="E42" t="s">
-        <v>107</v>
-      </c>
-      <c r="F42" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>100</v>
-      </c>
-      <c r="C43" t="s">
-        <v>105</v>
-      </c>
-      <c r="D43" t="s">
-        <v>103</v>
-      </c>
-      <c r="E43" t="s">
-        <v>108</v>
-      </c>
       <c r="F43" t="s">
+        <v>68</v>
+      </c>
+      <c r="G43" t="s">
+        <v>69</v>
+      </c>
+      <c r="H43" t="s">
         <v>8</v>
       </c>
-      <c r="G43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="F44" t="s">
+        <v>70</v>
+      </c>
+      <c r="G44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C47" t="s">
         <v>20</v>
@@ -1488,183 +1485,167 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C48" t="s">
         <v>23</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C49" t="s">
         <v>21</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
         <v>17</v>
       </c>
       <c r="D50" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
-      </c>
-      <c r="D51" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>56</v>
-      </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" t="s">
         <v>50</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F54" t="s">
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" t="s">
         <v>129</v>
       </c>
-      <c r="G54" t="s">
+      <c r="D57" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" t="s">
+        <v>133</v>
+      </c>
+      <c r="F57" t="s">
+        <v>131</v>
+      </c>
+      <c r="G57" t="s">
         <v>6</v>
       </c>
-      <c r="H54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>121</v>
-      </c>
-      <c r="C55" t="s">
-        <v>126</v>
-      </c>
-      <c r="D55" t="s">
-        <v>123</v>
-      </c>
-      <c r="E55" t="s">
-        <v>124</v>
-      </c>
-      <c r="F55" t="s">
-        <v>130</v>
-      </c>
-      <c r="G55" t="s">
+      <c r="H57" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" t="s">
+        <v>132</v>
+      </c>
+      <c r="E58" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" t="s">
+        <v>112</v>
+      </c>
+      <c r="G58" t="s">
         <v>7</v>
       </c>
-      <c r="H55" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" t="s">
-        <v>127</v>
-      </c>
-      <c r="D56" t="s">
-        <v>122</v>
-      </c>
-      <c r="E56" t="s">
-        <v>128</v>
-      </c>
-      <c r="F56" t="s">
-        <v>131</v>
-      </c>
-      <c r="G56" t="s">
-        <v>8</v>
-      </c>
-      <c r="H56" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" t="s">
-        <v>71</v>
-      </c>
-      <c r="E57" t="s">
-        <v>71</v>
-      </c>
-      <c r="F57" t="s">
-        <v>71</v>
+      <c r="H58" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>28</v>
-      </c>
-      <c r="D59" s="1">
-        <v>10</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>18</v>
+        <v>98</v>
+      </c>
+      <c r="D59" t="s">
+        <v>99</v>
+      </c>
+      <c r="E59" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" t="s">
+        <v>99</v>
+      </c>
+      <c r="G59" t="s">
+        <v>8</v>
+      </c>
+      <c r="H59" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>87</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
-      </c>
-      <c r="D60" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>113</v>
-      </c>
-      <c r="C61" t="s">
-        <v>29</v>
-      </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="D60" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C62" t="s">
         <v>28</v>
@@ -1672,190 +1653,259 @@
       <c r="D62" s="1">
         <v>10</v>
       </c>
-      <c r="E62" s="1"/>
+      <c r="E62" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s">
-        <v>21</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E63" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="D63" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F64" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="C65" t="s">
+        <v>148</v>
+      </c>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" t="s">
         <v>21</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>57</v>
-      </c>
-      <c r="B71" t="s">
-        <v>133</v>
-      </c>
-      <c r="C71" t="s">
-        <v>134</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>48</v>
+      </c>
+      <c r="C68" t="s">
+        <v>50</v>
+      </c>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" s="1">
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E70" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>46</v>
+      </c>
+      <c r="B74" t="s">
         <v>135</v>
       </c>
-      <c r="E71" t="s">
+      <c r="C74" t="s">
         <v>136</v>
       </c>
-      <c r="F71" t="s">
+      <c r="D74" t="s">
+        <v>138</v>
+      </c>
+      <c r="E74" t="s">
+        <v>142</v>
+      </c>
+      <c r="F74" t="s">
+        <v>144</v>
+      </c>
+      <c r="G74" t="s">
         <v>6</v>
       </c>
-      <c r="G71" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" t="s">
         <v>137</v>
       </c>
-      <c r="E72" t="s">
-        <v>138</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="D75" t="s">
+        <v>132</v>
+      </c>
+      <c r="E75" t="s">
+        <v>107</v>
+      </c>
+      <c r="F75" t="s">
+        <v>112</v>
+      </c>
+      <c r="G75" t="s">
         <v>7</v>
-      </c>
-      <c r="G72" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>122</v>
-      </c>
-      <c r="C73" t="s">
-        <v>128</v>
-      </c>
-      <c r="D73" t="s">
-        <v>139</v>
-      </c>
-      <c r="E73" t="s">
-        <v>139</v>
-      </c>
-      <c r="F73" t="s">
-        <v>8</v>
-      </c>
-      <c r="G73" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>1</v>
-      </c>
-      <c r="C74" t="s">
-        <v>3</v>
-      </c>
-      <c r="D74" t="s">
-        <v>2</v>
-      </c>
-      <c r="E74" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="C76" t="s">
-        <v>17</v>
-      </c>
-      <c r="D76" s="1">
-        <v>10</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>18</v>
+        <v>140</v>
+      </c>
+      <c r="D76" t="s">
+        <v>141</v>
+      </c>
+      <c r="E76" t="s">
+        <v>143</v>
+      </c>
+      <c r="F76" t="s">
+        <v>143</v>
+      </c>
+      <c r="G76" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>17</v>
-      </c>
-      <c r="D77" s="1">
-        <v>10</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>13</v>
-      </c>
-      <c r="C78" t="s">
-        <v>17</v>
-      </c>
-      <c r="D78" s="1">
-        <v>10</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>59</v>
+      </c>
+      <c r="E77" t="s">
+        <v>2</v>
+      </c>
+      <c r="F77" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="C79" t="s">
         <v>17</v>
       </c>
       <c r="D79" s="1">
-        <v>5</v>
-      </c>
-      <c r="E79" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
       <c r="C80" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" s="1">
+        <v>10</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" s="1">
+        <v>10</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>30</v>
+      </c>
+      <c r="C82" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="1">
+        <v>5</v>
+      </c>
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" t="s">
         <v>21</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E80" s="1"/>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>119</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="D83" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" t="s">
         <v>21</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>32</v>
+      <c r="D84" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Order Detail files
</commit_message>
<xml_diff>
--- a/Final Outputs/Schema and Workflow/ITECC05 SCHEMA.xlsx
+++ b/Final Outputs/Schema and Workflow/ITECC05 SCHEMA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamp\Desktop\ITECC05\itek05_collab\Final Outputs\Schema and Workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4482FF00-4CF0-4F66-AB41-6DD52FCF6F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE36B58-0449-47AA-93C3-3276919B0EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14955" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="151">
   <si>
     <t>db_food_kiosk</t>
   </si>
@@ -433,9 +433,6 @@
     <t>getDetailByOrderId</t>
   </si>
   <si>
-    <t>indexByOrder</t>
-  </si>
-  <si>
     <t>getDetailById</t>
   </si>
   <si>
@@ -473,6 +470,9 @@
   </si>
   <si>
     <t>NOT DONE</t>
+  </si>
+  <si>
+    <t>indexByOrderId</t>
   </si>
 </sst>
 </file>
@@ -796,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,675 +1190,658 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" t="s">
-        <v>150</v>
+        <v>62</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
         <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>44</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>117</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E30" t="s">
         <v>33</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F30" t="s">
         <v>32</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G30" t="s">
         <v>6</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H30" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C29" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" t="s">
-        <v>119</v>
-      </c>
-      <c r="F29" t="s">
-        <v>112</v>
-      </c>
-      <c r="G29" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" t="s">
-        <v>37</v>
-      </c>
-      <c r="G30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="E31" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="F31" t="s">
-        <v>2</v>
+        <v>112</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33">
-        <v>11</v>
+        <v>59</v>
+      </c>
+      <c r="D33" t="s">
+        <v>59</v>
       </c>
       <c r="E33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34">
-        <v>100</v>
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D35">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="D37">
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>49</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>76</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>121</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>123</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D43" t="s">
         <v>122</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E43" t="s">
         <v>87</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F43" t="s">
         <v>126</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G43" t="s">
         <v>127</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H43" t="s">
         <v>6</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I43" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" t="s">
-        <v>108</v>
-      </c>
-      <c r="D42" t="s">
-        <v>124</v>
-      </c>
-      <c r="E42" t="s">
-        <v>125</v>
-      </c>
-      <c r="F42" t="s">
-        <v>107</v>
-      </c>
-      <c r="G42" t="s">
-        <v>112</v>
-      </c>
-      <c r="H42" t="s">
-        <v>7</v>
-      </c>
-      <c r="I42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" t="s">
-        <v>86</v>
-      </c>
-      <c r="E43" t="s">
-        <v>88</v>
-      </c>
-      <c r="F43" t="s">
-        <v>68</v>
-      </c>
-      <c r="G43" t="s">
-        <v>69</v>
-      </c>
-      <c r="H43" t="s">
-        <v>8</v>
-      </c>
-      <c r="I43" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="E44" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="F44" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="G44" t="s">
-        <v>2</v>
+        <v>112</v>
+      </c>
+      <c r="H44" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" t="s">
+        <v>68</v>
+      </c>
+      <c r="G45" t="s">
+        <v>69</v>
+      </c>
+      <c r="H45" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="1">
-        <v>20</v>
+        <v>59</v>
+      </c>
+      <c r="D46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" t="s">
+        <v>59</v>
+      </c>
+      <c r="F46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G46" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C48" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>145</v>
+        <v>17</v>
+      </c>
+      <c r="D48" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D49" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="1">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
-      </c>
-      <c r="D52" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D52" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C53" t="s">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>49</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>45</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>128</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C59" t="s">
         <v>129</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E59" t="s">
         <v>133</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F59" t="s">
         <v>131</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G59" t="s">
         <v>6</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H59" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>106</v>
-      </c>
-      <c r="C58" t="s">
-        <v>108</v>
-      </c>
-      <c r="D58" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" t="s">
-        <v>107</v>
-      </c>
-      <c r="F58" t="s">
-        <v>112</v>
-      </c>
-      <c r="G58" t="s">
-        <v>7</v>
-      </c>
-      <c r="H58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>98</v>
-      </c>
-      <c r="C59" t="s">
-        <v>98</v>
-      </c>
-      <c r="D59" t="s">
-        <v>99</v>
-      </c>
-      <c r="E59" t="s">
-        <v>99</v>
-      </c>
-      <c r="F59" t="s">
-        <v>99</v>
-      </c>
-      <c r="G59" t="s">
-        <v>8</v>
-      </c>
-      <c r="H59" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C60" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="D60" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="E60" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="F60" t="s">
-        <v>134</v>
+        <v>112</v>
+      </c>
+      <c r="G60" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" t="s">
+        <v>99</v>
+      </c>
+      <c r="E61" t="s">
+        <v>99</v>
+      </c>
+      <c r="F61" t="s">
+        <v>99</v>
+      </c>
+      <c r="G61" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>28</v>
-      </c>
-      <c r="D62" s="1">
-        <v>10</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" t="s">
-        <v>20</v>
-      </c>
-      <c r="D63" s="1">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c r="D62" t="s">
+        <v>59</v>
+      </c>
+      <c r="E62" t="s">
+        <v>2</v>
+      </c>
+      <c r="F62" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="C64" t="s">
-        <v>83</v>
-      </c>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="D64" s="1">
+        <v>10</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>147</v>
+        <v>75</v>
       </c>
       <c r="C65" t="s">
-        <v>148</v>
-      </c>
-      <c r="E65" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="D65" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="C66" t="s">
-        <v>23</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D66" s="1"/>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="C67" t="s">
-        <v>21</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F67" s="1"/>
+        <v>147</v>
+      </c>
+      <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="C68" t="s">
-        <v>50</v>
+        <v>23</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="C69" t="s">
-        <v>28</v>
-      </c>
-      <c r="D69" s="1">
-        <v>10</v>
-      </c>
-      <c r="E69" t="s">
-        <v>149</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" t="s">
+        <v>50</v>
+      </c>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" t="s">
+        <v>28</v>
+      </c>
+      <c r="D71" s="1">
+        <v>10</v>
+      </c>
+      <c r="E71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>92</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C72" t="s">
         <v>21</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E70" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="E72" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>46</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B76" t="s">
         <v>135</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C76" t="s">
         <v>136</v>
       </c>
-      <c r="D74" t="s">
-        <v>138</v>
-      </c>
-      <c r="E74" t="s">
-        <v>142</v>
-      </c>
-      <c r="F74" t="s">
-        <v>144</v>
-      </c>
-      <c r="G74" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>106</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="D76" t="s">
         <v>137</v>
       </c>
-      <c r="D75" t="s">
-        <v>132</v>
-      </c>
-      <c r="E75" t="s">
-        <v>107</v>
-      </c>
-      <c r="F75" t="s">
-        <v>112</v>
-      </c>
-      <c r="G75" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>139</v>
-      </c>
-      <c r="C76" t="s">
-        <v>140</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>141</v>
-      </c>
-      <c r="E76" t="s">
-        <v>143</v>
       </c>
       <c r="F76" t="s">
         <v>143</v>
       </c>
       <c r="G76" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C77" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="D77" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="E77" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="F77" t="s">
-        <v>2</v>
+        <v>112</v>
+      </c>
+      <c r="G77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>138</v>
+      </c>
+      <c r="C78" t="s">
+        <v>139</v>
+      </c>
+      <c r="D78" t="s">
+        <v>140</v>
+      </c>
+      <c r="E78" t="s">
+        <v>142</v>
+      </c>
+      <c r="F78" t="s">
+        <v>142</v>
+      </c>
+      <c r="G78" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>17</v>
-      </c>
-      <c r="D79" s="1">
-        <v>10</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>27</v>
-      </c>
-      <c r="C80" t="s">
-        <v>17</v>
-      </c>
-      <c r="D80" s="1">
-        <v>10</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="D79" t="s">
+        <v>59</v>
+      </c>
+      <c r="E79" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="C81" t="s">
         <v>17</v>
@@ -1867,45 +1850,73 @@
         <v>10</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C82" t="s">
         <v>17</v>
       </c>
       <c r="D82" s="1">
-        <v>5</v>
-      </c>
-      <c r="E82" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="C83" t="s">
-        <v>21</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E83" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D83" s="1">
+        <v>10</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
+        <v>30</v>
+      </c>
+      <c r="C84" t="s">
+        <v>17</v>
+      </c>
+      <c r="D84" s="1">
+        <v>5</v>
+      </c>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>96</v>
+      </c>
+      <c r="C85" t="s">
+        <v>21</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>97</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C86" t="s">
         <v>21</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E84" s="1" t="s">
-        <v>150</v>
+      <c r="E86" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added validation in FoodItem files
</commit_message>
<xml_diff>
--- a/Final Outputs/Schema and Workflow/ITECC05 SCHEMA.xlsx
+++ b/Final Outputs/Schema and Workflow/ITECC05 SCHEMA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamp\Desktop\ITECC05\itek05_collab\Final Outputs\Schema and Workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE36B58-0449-47AA-93C3-3276919B0EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D0394D-7F86-436C-9391-6A34A44CAFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6105" yWindow="2760" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="151">
   <si>
     <t>db_food_kiosk</t>
   </si>
@@ -55,9 +55,6 @@
     <t>foodController</t>
   </si>
   <si>
-    <t>/api/foods</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -175,30 +172,15 @@
     <t>timestamp</t>
   </si>
   <si>
-    <t>/api/foods/:id</t>
-  </si>
-  <si>
     <t>/api/foods/remove/:id</t>
   </si>
   <si>
     <t>updateStock</t>
   </si>
   <si>
-    <t>/api/foods/stock/:id</t>
-  </si>
-  <si>
-    <t>/api/foods/available/:id</t>
-  </si>
-  <si>
     <t>getAvailableFood</t>
   </si>
   <si>
-    <t>/api/foods/available</t>
-  </si>
-  <si>
-    <t>/api/foods/category/:categoryId</t>
-  </si>
-  <si>
     <t xml:space="preserve">GET </t>
   </si>
   <si>
@@ -473,6 +455,24 @@
   </si>
   <si>
     <t>indexByOrderId</t>
+  </si>
+  <si>
+    <t>/api/fooditems</t>
+  </si>
+  <si>
+    <t>/api/fooditems/:foodId</t>
+  </si>
+  <si>
+    <t>/api/fooditems/available</t>
+  </si>
+  <si>
+    <t>/api/fooditems/category/:categoryId</t>
+  </si>
+  <si>
+    <t>/api/fooditems/stock/:foodId</t>
+  </si>
+  <si>
+    <t>/api/fooditems/available/:foodId</t>
   </si>
 </sst>
 </file>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,10 +809,10 @@
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" customWidth="1"/>
-    <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" customWidth="1"/>
@@ -828,34 +828,34 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
       </c>
       <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" t="s">
         <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" t="s">
-        <v>104</v>
       </c>
       <c r="K3" t="s">
         <v>6</v>
@@ -866,31 +866,31 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" t="s">
         <v>106</v>
-      </c>
-      <c r="C4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G4" t="s">
-        <v>107</v>
-      </c>
-      <c r="H4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" t="s">
-        <v>104</v>
       </c>
       <c r="K4" t="s">
         <v>7</v>
@@ -901,37 +901,37 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>148</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K5" t="s">
         <v>8</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -945,10 +945,10 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
         <v>2</v>
@@ -965,38 +965,36 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>100</v>
@@ -1005,22 +1003,22 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
       </c>
       <c r="D12" s="1">
         <v>11</v>
@@ -1029,10 +1027,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1041,20 +1039,20 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -1064,83 +1062,83 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H17" t="s">
         <v>6</v>
       </c>
       <c r="I17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" t="s">
         <v>106</v>
-      </c>
-      <c r="C18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" t="s">
-        <v>107</v>
-      </c>
-      <c r="G18" t="s">
-        <v>112</v>
       </c>
       <c r="H18" t="s">
         <v>7</v>
       </c>
       <c r="I18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G19" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
         <v>8</v>
       </c>
       <c r="I19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1148,16 +1146,16 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G20" t="s">
         <v>2</v>
@@ -1165,24 +1163,24 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22">
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -1190,10 +1188,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1201,96 +1199,96 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
       <c r="E26" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G30" t="s">
         <v>6</v>
       </c>
       <c r="H30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" t="s">
         <v>106</v>
-      </c>
-      <c r="C31" t="s">
-        <v>108</v>
-      </c>
-      <c r="D31" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" t="s">
-        <v>119</v>
-      </c>
-      <c r="F31" t="s">
-        <v>112</v>
       </c>
       <c r="G31" t="s">
         <v>7</v>
       </c>
       <c r="H31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" t="s">
         <v>36</v>
-      </c>
-      <c r="C32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" t="s">
-        <v>37</v>
       </c>
       <c r="G32" t="s">
         <v>8</v>
       </c>
       <c r="H32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1298,10 +1296,10 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
         <v>2</v>
@@ -1312,24 +1310,24 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35">
         <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36">
         <v>100</v>
@@ -1337,10 +1335,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D37">
         <v>15</v>
@@ -1348,10 +1346,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
@@ -1359,99 +1357,99 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
         <v>49</v>
-      </c>
-      <c r="C40" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" t="s">
+        <v>120</v>
+      </c>
+      <c r="G43" t="s">
         <v>121</v>
-      </c>
-      <c r="C43" t="s">
-        <v>123</v>
-      </c>
-      <c r="D43" t="s">
-        <v>122</v>
-      </c>
-      <c r="E43" t="s">
-        <v>87</v>
-      </c>
-      <c r="F43" t="s">
-        <v>126</v>
-      </c>
-      <c r="G43" t="s">
-        <v>127</v>
       </c>
       <c r="H43" t="s">
         <v>6</v>
       </c>
       <c r="I43" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" t="s">
+        <v>119</v>
+      </c>
+      <c r="F44" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" t="s">
         <v>106</v>
-      </c>
-      <c r="C44" t="s">
-        <v>108</v>
-      </c>
-      <c r="D44" t="s">
-        <v>124</v>
-      </c>
-      <c r="E44" t="s">
-        <v>125</v>
-      </c>
-      <c r="F44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G44" t="s">
-        <v>112</v>
       </c>
       <c r="H44" t="s">
         <v>7</v>
       </c>
       <c r="I44" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E45" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F45" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G45" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H45" t="s">
         <v>8</v>
       </c>
       <c r="I45" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -1459,16 +1457,16 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D46" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E46" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F46" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G46" t="s">
         <v>2</v>
@@ -1476,10 +1474,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D48" s="1">
         <v>11</v>
@@ -1487,10 +1485,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D49" s="1">
         <v>20</v>
@@ -1498,32 +1496,32 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C51" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D52" s="1">
         <v>11</v>
@@ -1531,10 +1529,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D53" s="1">
         <v>1</v>
@@ -1542,99 +1540,99 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C54" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" t="s">
         <v>49</v>
-      </c>
-      <c r="C56" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B59" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C59" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E59" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F59" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G59" t="s">
         <v>6</v>
       </c>
       <c r="H59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>100</v>
+      </c>
+      <c r="C60" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" t="s">
+        <v>101</v>
+      </c>
+      <c r="F60" t="s">
         <v>106</v>
-      </c>
-      <c r="C60" t="s">
-        <v>108</v>
-      </c>
-      <c r="D60" t="s">
-        <v>132</v>
-      </c>
-      <c r="E60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F60" t="s">
-        <v>112</v>
       </c>
       <c r="G60" t="s">
         <v>7</v>
       </c>
       <c r="H60" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C61" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D61" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E61" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F61" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G61" t="s">
         <v>8</v>
       </c>
       <c r="H61" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -1642,38 +1640,38 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D62" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E62" t="s">
         <v>2</v>
       </c>
       <c r="F62" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" t="s">
         <v>27</v>
-      </c>
-      <c r="C64" t="s">
-        <v>28</v>
       </c>
       <c r="D64" s="1">
         <v>10</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D65" s="1">
         <v>50</v>
@@ -1681,102 +1679,102 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C66" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C67" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C69" t="s">
+        <v>20</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C70" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D71" s="1">
         <v>10</v>
       </c>
       <c r="E71" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E72" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B76" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76" t="s">
+        <v>130</v>
+      </c>
+      <c r="D76" t="s">
+        <v>131</v>
+      </c>
+      <c r="E76" t="s">
         <v>135</v>
       </c>
-      <c r="C76" t="s">
-        <v>136</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="F76" t="s">
         <v>137</v>
-      </c>
-      <c r="E76" t="s">
-        <v>141</v>
-      </c>
-      <c r="F76" t="s">
-        <v>143</v>
       </c>
       <c r="G76" t="s">
         <v>6</v>
@@ -1784,19 +1782,19 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" t="s">
+        <v>144</v>
+      </c>
+      <c r="D77" t="s">
+        <v>126</v>
+      </c>
+      <c r="E77" t="s">
+        <v>101</v>
+      </c>
+      <c r="F77" t="s">
         <v>106</v>
-      </c>
-      <c r="C77" t="s">
-        <v>150</v>
-      </c>
-      <c r="D77" t="s">
-        <v>132</v>
-      </c>
-      <c r="E77" t="s">
-        <v>107</v>
-      </c>
-      <c r="F77" t="s">
-        <v>112</v>
       </c>
       <c r="G77" t="s">
         <v>7</v>
@@ -1804,19 +1802,19 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C78" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D78" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E78" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F78" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G78" t="s">
         <v>8</v>
@@ -1830,7 +1828,7 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E79" t="s">
         <v>2</v>
@@ -1841,52 +1839,52 @@
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D81" s="1">
         <v>10</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D82" s="1">
         <v>10</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D83" s="1">
         <v>10</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D84" s="1">
         <v>5</v>
@@ -1895,28 +1893,28 @@
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C86" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>